<commit_message>
(doc): journal de travail jour 1
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_MatKhalil-ops.xlsx
+++ b/Doc/Journal-de-Travail_MatKhalil-ops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pq40rdc\Documents\GitHub\PortofolioDev\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8086DF9F-5800-44F3-8B42-A7A19174A6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7555B431-D5C1-4A0B-BE01-6C1CBC1C40FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="6765" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Disscusion avec julien par rapport a la concesption du projet (schema au tableau)</t>
+  </si>
+  <si>
+    <t>chapitre intro du rapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analyse initale </t>
+  </si>
+  <si>
+    <t>workfile pour le testing et linting du code</t>
   </si>
 </sst>
 </file>
@@ -1158,13 +1167,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7.9861111111111105E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.1666666666666664E-2</c:v>
@@ -2092,7 +2101,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2145,7 +2154,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 0 minutes</v>
+        <v>0 jours 3 heurs 45 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2160,15 +2169,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2253,9 +2262,15 @@
       </c>
       <c r="B9" s="51"/>
       <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="37"/>
+      <c r="D9" s="53">
+        <v>20</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="18"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -2274,9 +2289,15 @@
       </c>
       <c r="B10" s="47"/>
       <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="49">
+        <v>30</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -2294,10 +2315,18 @@
         <v/>
       </c>
       <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="37"/>
+      <c r="C11" s="52">
+        <v>1</v>
+      </c>
+      <c r="D11" s="53">
+        <v>55</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="18"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -8735,11 +8764,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8747,7 +8776,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>7.9861111111111105E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8775,7 +8804,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8783,7 +8812,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8856,7 +8885,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9093,6 +9122,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9101,15 +9139,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9132,6 +9161,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9140,12 +9177,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>